<commit_message>
Work on the DisposeEqui patcher.
</commit_message>
<xml_diff>
--- a/DisposeEquiPatcher/excel-sample/Dispose_Equi_Worklist_Sample.xlsx
+++ b/DisposeEquiPatcher/excel-sample/Dispose_Equi_Worklist_Sample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\coding\work\asset-patch\DisposeEquiPatcher\excel-sample\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09A78E76-0D7D-44E5-93A3-F6F156EBDEAA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74AABF27-8387-4FFB-BE9C-1B8205027D32}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{65655A23-1E29-4E70-A082-B5F633D8CB57}"/>
   </bookViews>
@@ -31,10 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
-  <si>
-    <t>S4 Equipment</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
   <si>
     <t>Functional Location</t>
   </si>
@@ -100,6 +97,15 @@
   </si>
   <si>
     <t>Power Supply Unit 10</t>
+  </si>
+  <si>
+    <t>Object Type</t>
+  </si>
+  <si>
+    <t>PODE</t>
+  </si>
+  <si>
+    <t>S4 Equipment Id</t>
   </si>
 </sst>
 </file>
@@ -464,161 +470,195 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83161465-1FCA-41A2-BCF2-D6E72ABABA7E}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="48.28515625" customWidth="1"/>
-    <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="8" width="19" customWidth="1"/>
-    <col min="9" max="9" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.7109375" customWidth="1"/>
-    <col min="12" max="12" width="26.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21.140625" customWidth="1"/>
-    <col min="15" max="15" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="23.5703125" customWidth="1"/>
-    <col min="21" max="21" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="20.5703125" customWidth="1"/>
-    <col min="23" max="23" width="25.140625" customWidth="1"/>
-    <col min="24" max="24" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="20.5703125" customWidth="1"/>
-    <col min="26" max="26" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="23.85546875" customWidth="1"/>
-    <col min="28" max="28" width="52" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" customWidth="1"/>
+    <col min="3" max="3" width="48.28515625" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="19" customWidth="1"/>
+    <col min="10" max="10" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.7109375" customWidth="1"/>
+    <col min="13" max="13" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.140625" customWidth="1"/>
+    <col min="16" max="16" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="23.5703125" customWidth="1"/>
+    <col min="22" max="22" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="20.5703125" customWidth="1"/>
+    <col min="24" max="24" width="25.140625" customWidth="1"/>
+    <col min="25" max="25" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="20.5703125" customWidth="1"/>
+    <col min="27" max="27" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="23.85546875" customWidth="1"/>
+    <col min="29" max="29" width="52" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1000101001</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1000101002</v>
+      </c>
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1000101001</v>
-      </c>
-      <c r="B3" s="1" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1000101003</v>
+      </c>
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>1000101001</v>
-      </c>
-      <c r="B4" s="1" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1000101004</v>
+      </c>
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>1000101001</v>
-      </c>
-      <c r="B5" s="1" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1000101005</v>
+      </c>
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>1000101001</v>
-      </c>
-      <c r="B6" s="1" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1000101006</v>
+      </c>
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>1000101001</v>
-      </c>
-      <c r="B7" s="1" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1000101007</v>
+      </c>
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>1000101001</v>
-      </c>
-      <c r="B8" s="1" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1000101008</v>
+      </c>
+      <c r="B9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D9" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>1000101001</v>
-      </c>
-      <c r="B9" s="1" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>1000101009</v>
+      </c>
+      <c r="B10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>1000101001</v>
-      </c>
-      <c r="B10" s="1" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>1000101010</v>
+      </c>
+      <c r="B11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D11" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>1000101001</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added a CSV exporter for ChangeFiles.
</commit_message>
<xml_diff>
--- a/DisposeEquiPatcher/excel-sample/Dispose_Equi_Worklist_Sample.xlsx
+++ b/DisposeEquiPatcher/excel-sample/Dispose_Equi_Worklist_Sample.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\coding\work\asset-patch\DisposeEquiPatcher\excel-sample\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\coding\work\asset-patch\DisposeEquiPatcher\excel-sample\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74AABF27-8387-4FFB-BE9C-1B8205027D32}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D01976D0-EE2C-4383-B415-42405952EAE8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{65655A23-1E29-4E70-A082-B5F633D8CB57}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{65655A23-1E29-4E70-A082-B5F633D8CB57}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="29">
   <si>
     <t>Functional Location</t>
   </si>
@@ -106,6 +106,18 @@
   </si>
   <si>
     <t>S4 Equipment Id</t>
+  </si>
+  <si>
+    <t>Manufacturer</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>BattCo</t>
+  </si>
+  <si>
+    <t>Lithio 360</t>
   </si>
 </sst>
 </file>
@@ -470,20 +482,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83161465-1FCA-41A2-BCF2-D6E72ABABA7E}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.42578125" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="48.28515625" customWidth="1"/>
-    <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.42578125" customWidth="1"/>
     <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
     <col min="6" max="9" width="19" customWidth="1"/>
     <col min="10" max="10" width="25.140625" bestFit="1" customWidth="1"/>
@@ -507,158 +519,224 @@
     <col min="29" max="29" width="52" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>24</v>
       </c>
       <c r="B1" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="E1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1000101001</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="E2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1000101002</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="E3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1000101003</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="E4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1000101004</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="E5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1000101005</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="E6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1000101006</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="E7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1000101007</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="E8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1000101008</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="E9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1000101009</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="E10" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1000101010</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>21</v>
+        <v>23</v>
+      </c>
+      <c r="E11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F11" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Initial work towards ordering UXL equipment property updates - child equipment might need to be updated before the parent.
</commit_message>
<xml_diff>
--- a/DisposeEquiPatcher/excel-sample/Dispose_Equi_Worklist_Sample.xlsx
+++ b/DisposeEquiPatcher/excel-sample/Dispose_Equi_Worklist_Sample.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\coding\work\asset-patch\DisposeEquiPatcher\excel-sample\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\coding\work\asset-patch\DisposeEquiPatcher\excel-sample\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D01976D0-EE2C-4383-B415-42405952EAE8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F49945BF-E1AE-4C05-BFEA-A4E1B7A1B707}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{65655A23-1E29-4E70-A082-B5F633D8CB57}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{65655A23-1E29-4E70-A082-B5F633D8CB57}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="43">
   <si>
     <t>Functional Location</t>
   </si>
@@ -118,6 +118,48 @@
   </si>
   <si>
     <t>Lithio 360</t>
+  </si>
+  <si>
+    <t>Serial Number</t>
+  </si>
+  <si>
+    <t>Part Number</t>
+  </si>
+  <si>
+    <t>Superior Equipment</t>
+  </si>
+  <si>
+    <t>Status of an object</t>
+  </si>
+  <si>
+    <t>OPER</t>
+  </si>
+  <si>
+    <t>GMM-003</t>
+  </si>
+  <si>
+    <t>OBIE CZ</t>
+  </si>
+  <si>
+    <t>ZX81</t>
+  </si>
+  <si>
+    <t>ZX83</t>
+  </si>
+  <si>
+    <t>ZX84</t>
+  </si>
+  <si>
+    <t>ZX86</t>
+  </si>
+  <si>
+    <t>ZX87</t>
+  </si>
+  <si>
+    <t>ZX88</t>
+  </si>
+  <si>
+    <t>ZX90</t>
   </si>
 </sst>
 </file>
@@ -482,12 +524,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83161465-1FCA-41A2-BCF2-D6E72ABABA7E}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
+      <selection pane="bottomLeft" activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -519,7 +561,7 @@
     <col min="29" max="29" width="52" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -538,8 +580,20 @@
       <c r="F1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1000101001</v>
       </c>
@@ -558,8 +612,20 @@
       <c r="F2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H2" t="s">
+        <v>34</v>
+      </c>
+      <c r="I2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J2">
+        <v>1000100001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1000101002</v>
       </c>
@@ -578,8 +644,14 @@
       <c r="F3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I3" t="s">
+        <v>33</v>
+      </c>
+      <c r="J3">
+        <v>1000100001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1000101003</v>
       </c>
@@ -598,8 +670,17 @@
       <c r="F4" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" t="s">
+        <v>37</v>
+      </c>
+      <c r="I4" t="s">
+        <v>33</v>
+      </c>
+      <c r="J4">
+        <v>1000100001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1000101004</v>
       </c>
@@ -618,8 +699,17 @@
       <c r="F5" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" t="s">
+        <v>38</v>
+      </c>
+      <c r="H5" t="s">
+        <v>35</v>
+      </c>
+      <c r="I5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1000101005</v>
       </c>
@@ -638,8 +728,11 @@
       <c r="F6" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1000101006</v>
       </c>
@@ -658,8 +751,17 @@
       <c r="F7" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7" t="s">
+        <v>39</v>
+      </c>
+      <c r="I7" t="s">
+        <v>33</v>
+      </c>
+      <c r="J7">
+        <v>1000100002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1000101007</v>
       </c>
@@ -678,8 +780,17 @@
       <c r="F8" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8" t="s">
+        <v>40</v>
+      </c>
+      <c r="I8" t="s">
+        <v>33</v>
+      </c>
+      <c r="J8">
+        <v>1000100002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1000101008</v>
       </c>
@@ -698,8 +809,17 @@
       <c r="F9" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9" t="s">
+        <v>41</v>
+      </c>
+      <c r="I9" t="s">
+        <v>33</v>
+      </c>
+      <c r="J9">
+        <v>1000100002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1000101009</v>
       </c>
@@ -718,8 +838,11 @@
       <c r="F10" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1000101010</v>
       </c>
@@ -737,6 +860,12 @@
       </c>
       <c r="F11" t="s">
         <v>28</v>
+      </c>
+      <c r="G11" t="s">
+        <v>42</v>
+      </c>
+      <c r="I11" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>